<commit_message>
PDS4 Label creation code
</commit_message>
<xml_diff>
--- a/templates/Titan_UVIS_data_definition_v0.2.xlsx
+++ b/templates/Titan_UVIS_data_definition_v0.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotjp/git/fits_writer/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28690C42-07B2-0140-BB7C-7AB40B1B3F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4B015FC-8D89-6D43-AB32-0AA557FA2A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="L2A_product_definition" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Data types" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1725,8 +1726,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add description fields to Headers and all HDUs
Read the descriptions from the template spreadsheet and create appropriate XML elements.  Some code cleanup as well.
</commit_message>
<xml_diff>
--- a/templates/Titan_UVIS_data_definition_v0.2.xlsx
+++ b/templates/Titan_UVIS_data_definition_v0.2.xlsx
@@ -1,31 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotjp/git/fits_writer/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B4B015FC-8D89-6D43-AB32-0AA557FA2A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C10F015-3FD6-9C43-B700-012DF088B01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="L2A_product_definition" sheetId="1" r:id="rId1"/>
-    <sheet name="Level2-3 Sizes" sheetId="2" r:id="rId2"/>
-    <sheet name="Data types" sheetId="3" r:id="rId3"/>
+    <sheet name="HDU Descriptions" sheetId="4" r:id="rId2"/>
+    <sheet name="Level2-3 Sizes" sheetId="2" r:id="rId3"/>
+    <sheet name="Data types" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="302">
   <si>
     <t>HDU NAME</t>
   </si>
@@ -880,6 +878,66 @@
   </si>
   <si>
     <t>C_KRN</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Configuration Header</t>
+  </si>
+  <si>
+    <t>Information on instrument configuration</t>
+  </si>
+  <si>
+    <t>Rawcounts and calibrated UVIS data</t>
+  </si>
+  <si>
+    <t>2D arrays for each detector image in the FUV channel</t>
+  </si>
+  <si>
+    <t>This is the FITS header for the FOV_Geom HDU</t>
+  </si>
+  <si>
+    <t>Field Of View Geometry</t>
+  </si>
+  <si>
+    <t>This is the FITS header for the KERNELS HDU, which is list of all spice kernels used to compute geometry for this obsrevation</t>
+  </si>
+  <si>
+    <t>List of all kernels used to create the geomtrey</t>
+  </si>
+  <si>
+    <t>This is the FITS header for the SC_Geom HDU</t>
+  </si>
+  <si>
+    <t>Spacecraft Geometry</t>
+  </si>
+  <si>
+    <t>This is the FITS header for the Target_Geom HDU</t>
+  </si>
+  <si>
+    <t>Target Geometry</t>
+  </si>
+  <si>
+    <t>Time conversion from ET to UTC</t>
+  </si>
+  <si>
+    <t>This is the FITS header for the Wavelength HDU</t>
+  </si>
+  <si>
+    <t>Wavelength calibration for EUV or FUV channel</t>
+  </si>
+  <si>
+    <t>Calibration factor</t>
+  </si>
+  <si>
+    <t>UVIS data calibration matrix</t>
+  </si>
+  <si>
+    <t>2D arrays for each detector image in the EUV channel</t>
   </si>
 </sst>
 </file>
@@ -1726,8 +1784,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4706,6 +4764,158 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A910F-59B1-4B48-B27D-85A21AD25364}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="104.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C7" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" t="s">
+        <v>294</v>
+      </c>
+      <c r="C9" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B11" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12" t="s">
+        <v>301</v>
+      </c>
+      <c r="C12" t="s">
+        <v>301</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -4819,7 +5029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>

</xml_diff>

<commit_message>
Fixed spelling error in product def spreadsheet.
</commit_message>
<xml_diff>
--- a/templates/Titan_UVIS_data_definition_v0.2.xlsx
+++ b/templates/Titan_UVIS_data_definition_v0.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotjp/git/fits_writer/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C10F015-3FD6-9C43-B700-012DF088B01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519E7D21-6CDF-0440-BFD7-8AD5B3C1972F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="L2A_product_definition" sheetId="1" r:id="rId1"/>
@@ -892,9 +892,6 @@
     <t>Information on instrument configuration</t>
   </si>
   <si>
-    <t>Rawcounts and calibrated UVIS data</t>
-  </si>
-  <si>
     <t>2D arrays for each detector image in the FUV channel</t>
   </si>
   <si>
@@ -907,9 +904,6 @@
     <t>This is the FITS header for the KERNELS HDU, which is list of all spice kernels used to compute geometry for this obsrevation</t>
   </si>
   <si>
-    <t>List of all kernels used to create the geomtrey</t>
-  </si>
-  <si>
     <t>This is the FITS header for the SC_Geom HDU</t>
   </si>
   <si>
@@ -938,6 +932,12 @@
   </si>
   <si>
     <t>2D arrays for each detector image in the EUV channel</t>
+  </si>
+  <si>
+    <t>List of all kernels used to create the geometry</t>
+  </si>
+  <si>
+    <t>Raw counts and calibrated UVIS data</t>
   </si>
 </sst>
 </file>
@@ -4768,7 +4768,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4794,10 +4794,10 @@
         <v>277</v>
       </c>
       <c r="B2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C2" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -4816,10 +4816,10 @@
         <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -4827,10 +4827,10 @@
         <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -4838,10 +4838,10 @@
         <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="C6" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -4849,10 +4849,10 @@
         <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -4860,10 +4860,10 @@
         <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -4871,10 +4871,10 @@
         <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -4882,10 +4882,10 @@
         <v>161</v>
       </c>
       <c r="B10" t="s">
+        <v>287</v>
+      </c>
+      <c r="C10" t="s">
         <v>288</v>
-      </c>
-      <c r="C10" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -4893,10 +4893,10 @@
         <v>187</v>
       </c>
       <c r="B11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -4904,10 +4904,10 @@
         <v>203</v>
       </c>
       <c r="B12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C12" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>